<commit_message>
Se logo hacerlo andar pero no sé como hacer que el cursor se mueva
</commit_message>
<xml_diff>
--- a/5_TheRPAChallenge/challenge.xlsx
+++ b/5_TheRPAChallenge/challenge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calin.grigorescu\Documents\Projects\2021\Introduction to UI Automation\Modern Experience\Project\RPA Challenge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flopy\OneDrive\Documentos\UiPath\5_TheRPAChallenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195AEF2B-396D-4ADD-B06B-2F831947487C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB5169C-CEF7-492D-86E5-9C53AA095F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="13176" windowHeight="22656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -617,7 +617,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>